<commit_message>
roster.xlsx  - cleaned out test data  - added titles
</commit_message>
<xml_diff>
--- a/data/roster.xlsx
+++ b/data/roster.xlsx
@@ -5,16 +5,15 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilmo\OneDrive\Documents\aaaa\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilmo\Desktop\Veyon Class Builder\veyon-class-builder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{174F4DF5-EAE8-493A-A7CD-9A4B043BCB1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{79844DD4-5A4A-477F-A218-8AB1E72794D1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4CF879-3338-4CF3-BA97-BFF515C8EA2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E727EED-CB69-4603-B1A8-21FBD4712A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,18 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>a</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
+    <t>Hostname</t>
   </si>
 </sst>
 </file>
@@ -398,60 +391,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9876924D-D6D5-43D3-AE27-AD3A3F0F0C55}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:B3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>5678</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>3456</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195F444E-ADE7-4EAC-BFE7-0693241DF720}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data/export.txt  - blank slate  data/roster.xlsx  - blank slate  data/veyon_computers.txt  - blank slate
</commit_message>
<xml_diff>
--- a/data/roster.xlsx
+++ b/data/roster.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilmo\Desktop\Veyon Class Builder\veyon-class-builder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4CF879-3338-4CF3-BA97-BFF515C8EA2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F0CF1F-BF89-44FC-98FE-489497B46F9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E727EED-CB69-4603-B1A8-21FBD4712A20}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Class 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>